<commit_message>
added where to stream assigned movies to assignment
</commit_message>
<xml_diff>
--- a/class_materials/projects/movies/movies.xlsx
+++ b/class_materials/projects/movies/movies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emiliobruna/Dropbox (UFL)/Teaching/IDS 2935 - Future of Rain Forests/IDS2935_RainForests/class_materials/projects/movies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B33E26D-4581-2C48-8EF4-0DD74E4A544C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D310F88-76B6-F047-8E1F-45F48B24217B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="1540" windowWidth="18260" windowHeight="21100" xr2:uid="{353C7EC6-DCE5-5C40-B6C3-5F17E9D64295}"/>
+    <workbookView xWindow="10120" yWindow="3280" windowWidth="18260" windowHeight="21100" xr2:uid="{353C7EC6-DCE5-5C40-B6C3-5F17E9D64295}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="637">
   <si>
     <t>Tropic Thunder</t>
   </si>
@@ -7455,8 +7455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB7E5965-5A7E-9F4C-BD42-70F9C5F2FA16}">
   <dimension ref="A1:X141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C124" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
-      <selection activeCell="C129" sqref="C129"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7984,9 +7984,7 @@
       <c r="X14" s="2"/>
     </row>
     <row r="15" spans="1:24">
-      <c r="A15" s="4" t="s">
-        <v>620</v>
-      </c>
+      <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
         <v>362</v>
       </c>
@@ -9768,9 +9766,7 @@
       <c r="X65" s="2"/>
     </row>
     <row r="66" spans="1:24">
-      <c r="A66" s="4" t="s">
-        <v>620</v>
-      </c>
+      <c r="A66" s="4"/>
       <c r="B66" s="4" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
adding slides, updated syllabus
</commit_message>
<xml_diff>
--- a/class_materials/projects/movies/movies.xlsx
+++ b/class_materials/projects/movies/movies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emiliobruna/Dropbox (UFL)/Teaching/IDS 2935 - Future of Rain Forests/IDS2935_RainForests/class_materials/projects/movies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D310F88-76B6-F047-8E1F-45F48B24217B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9F9073-FBC6-C742-8B8E-5F2A0A268551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10120" yWindow="3280" windowWidth="18260" windowHeight="21100" xr2:uid="{353C7EC6-DCE5-5C40-B6C3-5F17E9D64295}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="637">
   <si>
     <t>Tropic Thunder</t>
   </si>
@@ -7455,8 +7455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB7E5965-5A7E-9F4C-BD42-70F9C5F2FA16}">
   <dimension ref="A1:X141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView tabSelected="1" topLeftCell="D3" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7995,7 +7995,9 @@
         <v>1951</v>
       </c>
       <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+      <c r="F15" s="4" t="s">
+        <v>327</v>
+      </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>

</xml_diff>